<commit_message>
Change example data for factor analysis
</commit_message>
<xml_diff>
--- a/covid19_drdfm/data/example-output/AK/df.xlsx
+++ b/covid19_drdfm/data/example-output/AK/df.xlsx
@@ -447,22 +447,22 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Employment1</t>
+          <t>GDP</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Employment2</t>
+          <t>Prod</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>CPIU</t>
+          <t>UI</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>PCEC</t>
+          <t>UR</t>
         </is>
       </c>
     </row>
@@ -471,16 +471,16 @@
         <v>40940</v>
       </c>
       <c r="B2" t="n">
-        <v>0.8170711884503437</v>
+        <v>0.6164068416721536</v>
       </c>
       <c r="C2" t="n">
-        <v>0.8237297960071758</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D2" t="n">
-        <v>0.4804248097350872</v>
+        <v>0.1440860989987424</v>
       </c>
       <c r="E2" t="n">
-        <v>0.5326596147660031</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="3">
@@ -488,16 +488,16 @@
         <v>40969</v>
       </c>
       <c r="B3" t="n">
-        <v>0.8135122768330407</v>
+        <v>0.621369126268051</v>
       </c>
       <c r="C3" t="n">
-        <v>0.8217942005629378</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D3" t="n">
-        <v>0.4783596646895119</v>
+        <v>0.1122897721076911</v>
       </c>
       <c r="E3" t="n">
-        <v>0.5620844651853298</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="4">
@@ -505,16 +505,16 @@
         <v>41000</v>
       </c>
       <c r="B4" t="n">
-        <v>0.8018882440272991</v>
+        <v>0.6823715730082882</v>
       </c>
       <c r="C4" t="n">
-        <v>0.8158387327196476</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D4" t="n">
-        <v>0.4580164258916395</v>
+        <v>0.1074542998569336</v>
       </c>
       <c r="E4" t="n">
-        <v>0.5446525784407911</v>
+        <v>0.3866666666666666</v>
       </c>
     </row>
     <row r="5">
@@ -522,16 +522,16 @@
         <v>41030</v>
       </c>
       <c r="B5" t="n">
-        <v>0.8182644828456356</v>
+        <v>0.7201480508129824</v>
       </c>
       <c r="C5" t="n">
-        <v>0.8168747967004858</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D5" t="n">
-        <v>0.2823120937051792</v>
+        <v>0.05512905676990382</v>
       </c>
       <c r="E5" t="n">
-        <v>0.496823265987087</v>
+        <v>0.3866666666666666</v>
       </c>
     </row>
     <row r="6">
@@ -539,16 +539,16 @@
         <v>41061</v>
       </c>
       <c r="B6" t="n">
-        <v>0.8137537407112719</v>
+        <v>0.7105015615464281</v>
       </c>
       <c r="C6" t="n">
-        <v>0.8153773111977091</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D6" t="n">
-        <v>0.3408982227867237</v>
+        <v>0.1015260822542131</v>
       </c>
       <c r="E6" t="n">
-        <v>0.4986300050073535</v>
+        <v>0.3866666666666666</v>
       </c>
     </row>
     <row r="7">
@@ -556,16 +556,16 @@
         <v>41091</v>
       </c>
       <c r="B7" t="n">
-        <v>0.8032999920192481</v>
+        <v>0.6525811755071577</v>
       </c>
       <c r="C7" t="n">
-        <v>0.8184443536062311</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D7" t="n">
-        <v>0.3934463727922193</v>
+        <v>0.09407286549104771</v>
       </c>
       <c r="E7" t="n">
-        <v>0.4985300066268447</v>
+        <v>0.3733333333333333</v>
       </c>
     </row>
     <row r="8">
@@ -573,16 +573,16 @@
         <v>41122</v>
       </c>
       <c r="B8" t="n">
-        <v>0.8069065484055066</v>
+        <v>0.6060805420880557</v>
       </c>
       <c r="C8" t="n">
-        <v>0.8197213812617881</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D8" t="n">
-        <v>0.6527359268372354</v>
+        <v>0.13148584303806</v>
       </c>
       <c r="E8" t="n">
-        <v>0.4604388239024145</v>
+        <v>0.3733333333333333</v>
       </c>
     </row>
     <row r="9">
@@ -590,16 +590,16 @@
         <v>41153</v>
       </c>
       <c r="B9" t="n">
-        <v>0.834591805387279</v>
+        <v>0.6109846329278866</v>
       </c>
       <c r="C9" t="n">
-        <v>0.8199184598513599</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D9" t="n">
-        <v>0.6040928049754837</v>
+        <v>0.1072413132675408</v>
       </c>
       <c r="E9" t="n">
-        <v>0.518296328753786</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="10">
@@ -607,16 +607,16 @@
         <v>41183</v>
       </c>
       <c r="B10" t="n">
-        <v>0.8210965500458856</v>
+        <v>0.5879194573625603</v>
       </c>
       <c r="C10" t="n">
-        <v>0.8189585210915629</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D10" t="n">
-        <v>0.506728251696605</v>
+        <v>0.1979392916345319</v>
       </c>
       <c r="E10" t="n">
-        <v>0.6299096914841315</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="11">
@@ -624,16 +624,16 @@
         <v>41214</v>
       </c>
       <c r="B11" t="n">
-        <v>0.8033629658599835</v>
+        <v>0.6442164614911825</v>
       </c>
       <c r="C11" t="n">
-        <v>0.8191157606636335</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D11" t="n">
-        <v>0.3006557725101743</v>
+        <v>0.3061360621220456</v>
       </c>
       <c r="E11" t="n">
-        <v>0.5036900929811654</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="12">
@@ -641,16 +641,16 @@
         <v>41244</v>
       </c>
       <c r="B12" t="n">
-        <v>0.8068337204551878</v>
+        <v>0.6359996657102006</v>
       </c>
       <c r="C12" t="n">
-        <v>0.8223201170577645</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D12" t="n">
-        <v>0.37413804795302</v>
+        <v>0.2255652297550041</v>
       </c>
       <c r="E12" t="n">
-        <v>0.4695708660232183</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="13">
@@ -658,16 +658,16 @@
         <v>41275</v>
       </c>
       <c r="B13" t="n">
-        <v>0.8055543580226956</v>
+        <v>0.6770921850179689</v>
       </c>
       <c r="C13" t="n">
-        <v>0.8202058936939317</v>
+        <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>0.4730736920152049</v>
+        <v>0.2280251376141953</v>
       </c>
       <c r="E13" t="n">
-        <v>0.59595739971971</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="14">
@@ -675,16 +675,16 @@
         <v>41306</v>
       </c>
       <c r="B14" t="n">
-        <v>0.8095017709632395</v>
+        <v>0.6502556855926304</v>
       </c>
       <c r="C14" t="n">
-        <v>0.8238479088897778</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D14" t="n">
-        <v>0.6349860070635606</v>
+        <v>0.06453636226351153</v>
       </c>
       <c r="E14" t="n">
-        <v>0.5145989657672945</v>
+        <v>0.3466666666666667</v>
       </c>
     </row>
     <row r="15">
@@ -692,16 +692,16 @@
         <v>41334</v>
       </c>
       <c r="B15" t="n">
-        <v>0.805262264353838</v>
+        <v>0.7273742772258296</v>
       </c>
       <c r="C15" t="n">
-        <v>0.8183347319329395</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D15" t="n">
-        <v>0.2471689513070562</v>
+        <v>0.124020122677636</v>
       </c>
       <c r="E15" t="n">
-        <v>0.4881206313599965</v>
+        <v>0.3466666666666667</v>
       </c>
     </row>
     <row r="16">
@@ -709,16 +709,16 @@
         <v>41365</v>
       </c>
       <c r="B16" t="n">
-        <v>0.8185903306715626</v>
+        <v>0.5873098952179144</v>
       </c>
       <c r="C16" t="n">
-        <v>0.8200477520852829</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D16" t="n">
-        <v>0.2813645162752761</v>
+        <v>0.101632600596866</v>
       </c>
       <c r="E16" t="n">
-        <v>0.4739383917639158</v>
+        <v>0.3466666666666667</v>
       </c>
     </row>
     <row r="17">
@@ -726,16 +726,16 @@
         <v>41395</v>
       </c>
       <c r="B17" t="n">
-        <v>0.815943793632123</v>
+        <v>0.5641802033850231</v>
       </c>
       <c r="C17" t="n">
-        <v>0.8211815955429621</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D17" t="n">
-        <v>0.3993518297214528</v>
+        <v>0.08932505371864924</v>
       </c>
       <c r="E17" t="n">
-        <v>0.5030030922048085</v>
+        <v>0.3466666666666667</v>
       </c>
     </row>
     <row r="18">
@@ -743,16 +743,16 @@
         <v>41426</v>
       </c>
       <c r="B18" t="n">
-        <v>0.8112013334931283</v>
+        <v>0.5400082867983307</v>
       </c>
       <c r="C18" t="n">
-        <v>0.8196578374857798</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D18" t="n">
-        <v>0.4918638127890506</v>
+        <v>0.1089233083405809</v>
       </c>
       <c r="E18" t="n">
-        <v>0.5563584867112221</v>
+        <v>0.3466666666666667</v>
       </c>
     </row>
     <row r="19">
@@ -760,16 +760,16 @@
         <v>41456</v>
       </c>
       <c r="B19" t="n">
-        <v>0.8165747062094404</v>
+        <v>0.7805034209619559</v>
       </c>
       <c r="C19" t="n">
-        <v>0.8173653310839419</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D19" t="n">
-        <v>0.4719810427311055</v>
+        <v>0.0586162568637577</v>
       </c>
       <c r="E19" t="n">
-        <v>0.5214607516946247</v>
+        <v>0.3466666666666667</v>
       </c>
     </row>
     <row r="20">
@@ -777,16 +777,16 @@
         <v>41487</v>
       </c>
       <c r="B20" t="n">
-        <v>0.8091941800468382</v>
+        <v>0.7751568136713394</v>
       </c>
       <c r="C20" t="n">
-        <v>0.8223289524283204</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D20" t="n">
-        <v>0.4921920362000497</v>
+        <v>0.1261853285195023</v>
       </c>
       <c r="E20" t="n">
-        <v>0.5110193252715993</v>
+        <v>0.3466666666666667</v>
       </c>
     </row>
     <row r="21">
@@ -794,16 +794,16 @@
         <v>41518</v>
       </c>
       <c r="B21" t="n">
-        <v>0.8102815037840168</v>
+        <v>0.7921401658634863</v>
       </c>
       <c r="C21" t="n">
-        <v>0.8198728129715163</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D21" t="n">
-        <v>0.3976005690238599</v>
+        <v>0.0963279929210932</v>
       </c>
       <c r="E21" t="n">
-        <v>0.5071548713574783</v>
+        <v>0.3466666666666667</v>
       </c>
     </row>
     <row r="22">
@@ -811,16 +811,16 @@
         <v>41548</v>
       </c>
       <c r="B22" t="n">
-        <v>0.7748893508307949</v>
+        <v>0.5602705796001579</v>
       </c>
       <c r="C22" t="n">
-        <v>0.8213239601066769</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D22" t="n">
-        <v>0.4050553748719518</v>
+        <v>0.2421768902759835</v>
       </c>
       <c r="E22" t="n">
-        <v>0.6021948355235164</v>
+        <v>0.3466666666666667</v>
       </c>
     </row>
     <row r="23">
@@ -828,16 +828,16 @@
         <v>41579</v>
       </c>
       <c r="B23" t="n">
-        <v>0.8412095355145293</v>
+        <v>0.5616119572896627</v>
       </c>
       <c r="C23" t="n">
-        <v>0.8235377070539099</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D23" t="n">
-        <v>0.4666731454969064</v>
+        <v>0.2947229178095876</v>
       </c>
       <c r="E23" t="n">
-        <v>0.5673374963087496</v>
+        <v>0.3333333333333334</v>
       </c>
     </row>
     <row r="24">
@@ -845,16 +845,16 @@
         <v>41609</v>
       </c>
       <c r="B24" t="n">
-        <v>0.8177730833014433</v>
+        <v>0.5542663252114519</v>
       </c>
       <c r="C24" t="n">
-        <v>0.8145750700290521</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D24" t="n">
-        <v>0.504271433281398</v>
+        <v>0.194697418949688</v>
       </c>
       <c r="E24" t="n">
-        <v>0.5298720316666941</v>
+        <v>0.3333333333333334</v>
       </c>
     </row>
     <row r="25">
@@ -862,16 +862,16 @@
         <v>41640</v>
       </c>
       <c r="B25" t="n">
-        <v>0.8203859482666936</v>
+        <v>0.6771956025949474</v>
       </c>
       <c r="C25" t="n">
-        <v>0.8198329027452651</v>
+        <v>0.6901305918451194</v>
       </c>
       <c r="D25" t="n">
-        <v>0.493934346505972</v>
+        <v>0.1804486979513476</v>
       </c>
       <c r="E25" t="n">
-        <v>0.4869849820012342</v>
+        <v>0.3333333333333334</v>
       </c>
     </row>
     <row r="26">
@@ -879,16 +879,16 @@
         <v>41671</v>
       </c>
       <c r="B26" t="n">
-        <v>0.8063658967333401</v>
+        <v>0.6975406611789488</v>
       </c>
       <c r="C26" t="n">
-        <v>0.8186518557405352</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D26" t="n">
-        <v>0.4316850960443767</v>
+        <v>0.1270476704292116</v>
       </c>
       <c r="E26" t="n">
-        <v>0.4590656589206957</v>
+        <v>0.3333333333333334</v>
       </c>
     </row>
     <row r="27">
@@ -896,16 +896,16 @@
         <v>41699</v>
       </c>
       <c r="B27" t="n">
-        <v>0.8254627173521412</v>
+        <v>0.6755643557920494</v>
       </c>
       <c r="C27" t="n">
-        <v>0.8236449003660327</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D27" t="n">
-        <v>0.4759716818008413</v>
+        <v>0.1201335951540758</v>
       </c>
       <c r="E27" t="n">
-        <v>0.5813985852189747</v>
+        <v>0.3333333333333334</v>
       </c>
     </row>
     <row r="28">
@@ -913,16 +913,16 @@
         <v>41730</v>
       </c>
       <c r="B28" t="n">
-        <v>0.8076266774238325</v>
+        <v>0.7029687401246343</v>
       </c>
       <c r="C28" t="n">
-        <v>0.8249493924630638</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D28" t="n">
-        <v>0.467607911577312</v>
+        <v>0.07921217235477812</v>
       </c>
       <c r="E28" t="n">
-        <v>0.5810588211558567</v>
+        <v>0.3333333333333334</v>
       </c>
     </row>
     <row r="29">
@@ -930,16 +930,16 @@
         <v>41760</v>
       </c>
       <c r="B29" t="n">
-        <v>0.8126222115907127</v>
+        <v>0.706220521880068</v>
       </c>
       <c r="C29" t="n">
-        <v>0.8205458782403786</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D29" t="n">
-        <v>0.4694354679379368</v>
+        <v>0.1012240624208627</v>
       </c>
       <c r="E29" t="n">
-        <v>0.568720941497564</v>
+        <v>0.3333333333333334</v>
       </c>
     </row>
     <row r="30">
@@ -947,16 +947,16 @@
         <v>41791</v>
       </c>
       <c r="B30" t="n">
-        <v>0.822080809866217</v>
+        <v>0.7153292372930169</v>
       </c>
       <c r="C30" t="n">
-        <v>0.8257039822361284</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D30" t="n">
-        <v>0.4420601940130754</v>
+        <v>0.1042910032867682</v>
       </c>
       <c r="E30" t="n">
-        <v>0.510356571489772</v>
+        <v>0.3333333333333334</v>
       </c>
     </row>
     <row r="31">
@@ -964,16 +964,16 @@
         <v>41821</v>
       </c>
       <c r="B31" t="n">
-        <v>0.8123850160291054</v>
+        <v>0.6111041377250467</v>
       </c>
       <c r="C31" t="n">
-        <v>0.8221142682634116</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D31" t="n">
-        <v>0.4328522352647602</v>
+        <v>0.07000526180675472</v>
       </c>
       <c r="E31" t="n">
-        <v>0.5746783049379056</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="32">
@@ -981,16 +981,16 @@
         <v>41852</v>
       </c>
       <c r="B32" t="n">
-        <v>0.8116286777528561</v>
+        <v>0.6361962443248149</v>
       </c>
       <c r="C32" t="n">
-        <v>0.8196616635690087</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D32" t="n">
-        <v>0.3723022077765162</v>
+        <v>0.111449767111071</v>
       </c>
       <c r="E32" t="n">
-        <v>0.4364593754966282</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="33">
@@ -998,16 +998,16 @@
         <v>41883</v>
       </c>
       <c r="B33" t="n">
-        <v>0.8158018120719297</v>
+        <v>0.6301351633293351</v>
       </c>
       <c r="C33" t="n">
-        <v>0.8245558462563858</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D33" t="n">
-        <v>0.3832166305801797</v>
+        <v>0.09578990577042812</v>
       </c>
       <c r="E33" t="n">
-        <v>0.5182623051006804</v>
+        <v>0.3066666666666666</v>
       </c>
     </row>
     <row r="34">
@@ -1015,16 +1015,16 @@
         <v>41913</v>
       </c>
       <c r="B34" t="n">
-        <v>0.8300547056264846</v>
+        <v>0.5295629292596407</v>
       </c>
       <c r="C34" t="n">
-        <v>0.8220236597927636</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D34" t="n">
-        <v>0.3705152434098531</v>
+        <v>0.17172887274119</v>
       </c>
       <c r="E34" t="n">
-        <v>0.4859909825289625</v>
+        <v>0.28</v>
       </c>
     </row>
     <row r="35">
@@ -1032,16 +1032,16 @@
         <v>41944</v>
       </c>
       <c r="B35" t="n">
-        <v>0.8061260573769912</v>
+        <v>0.5357992890571851</v>
       </c>
       <c r="C35" t="n">
-        <v>0.8236746516212029</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D35" t="n">
-        <v>0.2910385964014466</v>
+        <v>0.2772965514400872</v>
       </c>
       <c r="E35" t="n">
-        <v>0.5024243733665575</v>
+        <v>0.2666666666666667</v>
       </c>
     </row>
     <row r="36">
@@ -1049,16 +1049,16 @@
         <v>41974</v>
       </c>
       <c r="B36" t="n">
-        <v>0.8144364776464362</v>
+        <v>0.5459360694544858</v>
       </c>
       <c r="C36" t="n">
-        <v>0.8233744488067245</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D36" t="n">
-        <v>0.2342588880723614</v>
+        <v>0.2158126148065936</v>
       </c>
       <c r="E36" t="n">
-        <v>0.4894897771821189</v>
+        <v>0.2533333333333333</v>
       </c>
     </row>
     <row r="37">
@@ -1066,16 +1066,16 @@
         <v>42005</v>
       </c>
       <c r="B37" t="n">
-        <v>0.8257177919739254</v>
+        <v>0.4933860342845025</v>
       </c>
       <c r="C37" t="n">
-        <v>0.8201488230902793</v>
+        <v>0.8591709228043908</v>
       </c>
       <c r="D37" t="n">
-        <v>0.07870096975326518</v>
+        <v>0.1607343666376183</v>
       </c>
       <c r="E37" t="n">
-        <v>0.3813286191733929</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="38">
@@ -1083,16 +1083,16 @@
         <v>42036</v>
       </c>
       <c r="B38" t="n">
-        <v>0.8034061642763356</v>
+        <v>0.3913327842232263</v>
       </c>
       <c r="C38" t="n">
-        <v>0.8229426152859306</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D38" t="n">
-        <v>0.4991270461619542</v>
+        <v>0.1319021989761222</v>
       </c>
       <c r="E38" t="n">
-        <v>0.4958342593224085</v>
+        <v>0.2533333333333333</v>
       </c>
     </row>
     <row r="39">
@@ -1100,16 +1100,16 @@
         <v>42064</v>
       </c>
       <c r="B39" t="n">
-        <v>0.8098794065368862</v>
+        <v>0.3822867495056693</v>
       </c>
       <c r="C39" t="n">
-        <v>0.8161387989449225</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D39" t="n">
-        <v>0.5066174053952723</v>
+        <v>0.1190369140199784</v>
       </c>
       <c r="E39" t="n">
-        <v>0.5469451477989283</v>
+        <v>0.2533333333333333</v>
       </c>
     </row>
     <row r="40">
@@ -1117,16 +1117,16 @@
         <v>42095</v>
       </c>
       <c r="B40" t="n">
-        <v>0.8204703357769915</v>
+        <v>0.6819479128400981</v>
       </c>
       <c r="C40" t="n">
-        <v>0.8233488059890725</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D40" t="n">
-        <v>0.4289422565245661</v>
+        <v>0.07275719059816861</v>
       </c>
       <c r="E40" t="n">
-        <v>0.5613252734707689</v>
+        <v>0.2533333333333333</v>
       </c>
     </row>
     <row r="41">
@@ -1134,16 +1134,16 @@
         <v>42125</v>
       </c>
       <c r="B41" t="n">
-        <v>0.8177257676594207</v>
+        <v>0.656809246632998</v>
       </c>
       <c r="C41" t="n">
-        <v>0.8256853374382761</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D41" t="n">
-        <v>0.5349905266530876</v>
+        <v>0.05308076206967416</v>
       </c>
       <c r="E41" t="n">
-        <v>0.5182261974851207</v>
+        <v>0.2533333333333333</v>
       </c>
     </row>
     <row r="42">
@@ -1151,16 +1151,16 @@
         <v>42156</v>
       </c>
       <c r="B42" t="n">
-        <v>0.8069081625681082</v>
+        <v>0.6638021090385847</v>
       </c>
       <c r="C42" t="n">
-        <v>0.8184754748785685</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D42" t="n">
-        <v>0.5101022712614719</v>
+        <v>0.1240000415842817</v>
       </c>
       <c r="E42" t="n">
-        <v>0.5153510997590612</v>
+        <v>0.2533333333333333</v>
       </c>
     </row>
     <row r="43">
@@ -1168,16 +1168,16 @@
         <v>42186</v>
       </c>
       <c r="B43" t="n">
-        <v>0.8074361484750139</v>
+        <v>0.5757505992860273</v>
       </c>
       <c r="C43" t="n">
-        <v>0.8239159639196696</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D43" t="n">
-        <v>0.4545412938591608</v>
+        <v>0.06637858167142739</v>
       </c>
       <c r="E43" t="n">
-        <v>0.4842923898420154</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="44">
@@ -1185,16 +1185,16 @@
         <v>42217</v>
       </c>
       <c r="B44" t="n">
-        <v>0.8192830710681206</v>
+        <v>0.5877020937600063</v>
       </c>
       <c r="C44" t="n">
-        <v>0.8179084431114235</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D44" t="n">
-        <v>0.3796449961608567</v>
+        <v>0.1354541324196869</v>
       </c>
       <c r="E44" t="n">
-        <v>0.4696773108866913</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="45">
@@ -1202,16 +1202,16 @@
         <v>42248</v>
       </c>
       <c r="B45" t="n">
-        <v>0.7944628639571398</v>
+        <v>0.6101593227730051</v>
       </c>
       <c r="C45" t="n">
-        <v>0.8176684171428668</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D45" t="n">
-        <v>0.2738033829246919</v>
+        <v>0.1258471948126747</v>
       </c>
       <c r="E45" t="n">
-        <v>0.5232024759275713</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="46">
@@ -1219,16 +1219,16 @@
         <v>42278</v>
       </c>
       <c r="B46" t="n">
-        <v>0.8217058068666531</v>
+        <v>0.6166005006397922</v>
       </c>
       <c r="C46" t="n">
-        <v>0.8248840524521739</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D46" t="n">
-        <v>0.4264502145385787</v>
+        <v>0.239331943070692</v>
       </c>
       <c r="E46" t="n">
-        <v>0.4141878618902529</v>
+        <v>0.2533333333333333</v>
       </c>
     </row>
     <row r="47">
@@ -1236,16 +1236,16 @@
         <v>42309</v>
       </c>
       <c r="B47" t="n">
-        <v>0.8145543568902583</v>
+        <v>0.6045189410425847</v>
       </c>
       <c r="C47" t="n">
-        <v>0.8211576163575424</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D47" t="n">
-        <v>0.4361074937639563</v>
+        <v>0.2982344488436959</v>
       </c>
       <c r="E47" t="n">
-        <v>0.501270068544386</v>
+        <v>0.2533333333333333</v>
       </c>
     </row>
     <row r="48">
@@ -1253,16 +1253,16 @@
         <v>42339</v>
       </c>
       <c r="B48" t="n">
-        <v>0.8301987447499016</v>
+        <v>0.6262390898640361</v>
       </c>
       <c r="C48" t="n">
-        <v>0.8230098564771564</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D48" t="n">
-        <v>0.3291286649421136</v>
+        <v>0.2411146563540022</v>
       </c>
       <c r="E48" t="n">
-        <v>0.4631148953474943</v>
+        <v>0.2666666666666667</v>
       </c>
     </row>
     <row r="49">
@@ -1270,16 +1270,16 @@
         <v>42370</v>
       </c>
       <c r="B49" t="n">
-        <v>0.8252302269764712</v>
+        <v>0.6218268913301505</v>
       </c>
       <c r="C49" t="n">
-        <v>0.8168565564594282</v>
+        <v>0.774400728555791</v>
       </c>
       <c r="D49" t="n">
-        <v>0.3582333302100829</v>
+        <v>0.1810869781882656</v>
       </c>
       <c r="E49" t="n">
-        <v>0.5771039990911292</v>
+        <v>0.2666666666666667</v>
       </c>
     </row>
     <row r="50">
@@ -1287,16 +1287,16 @@
         <v>42401</v>
       </c>
       <c r="B50" t="n">
-        <v>0.8168785545332913</v>
+        <v>0.6391815304710607</v>
       </c>
       <c r="C50" t="n">
-        <v>0.8206159793291865</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D50" t="n">
-        <v>0.317139331932879</v>
+        <v>0.1450492108969805</v>
       </c>
       <c r="E50" t="n">
-        <v>0.5496922337370033</v>
+        <v>0.28</v>
       </c>
     </row>
     <row r="51">
@@ -1304,16 +1304,16 @@
         <v>42430</v>
       </c>
       <c r="B51" t="n">
-        <v>0.8166172624762037</v>
+        <v>0.5934462590949157</v>
       </c>
       <c r="C51" t="n">
-        <v>0.8223074009416873</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D51" t="n">
-        <v>0.527342817213182</v>
+        <v>0.1168125513883238</v>
       </c>
       <c r="E51" t="n">
-        <v>0.5377388043426896</v>
+        <v>0.28</v>
       </c>
     </row>
     <row r="52">
@@ -1321,16 +1321,16 @@
         <v>42461</v>
       </c>
       <c r="B52" t="n">
-        <v>0.8019526135529373</v>
+        <v>0.7080970658943831</v>
       </c>
       <c r="C52" t="n">
-        <v>0.8197387300407529</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D52" t="n">
-        <v>0.5600276253743403</v>
+        <v>0.09495281366725412</v>
       </c>
       <c r="E52" t="n">
-        <v>0.6392441489619071</v>
+        <v>0.28</v>
       </c>
     </row>
     <row r="53">
@@ -1338,16 +1338,16 @@
         <v>42491</v>
       </c>
       <c r="B53" t="n">
-        <v>0.8089540979698909</v>
+        <v>0.7359868866891046</v>
       </c>
       <c r="C53" t="n">
-        <v>0.8141278214900715</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D53" t="n">
-        <v>0.4911291353516724</v>
+        <v>0.08060951510601597</v>
       </c>
       <c r="E53" t="n">
-        <v>0.5461856617431168</v>
+        <v>0.2933333333333332</v>
       </c>
     </row>
     <row r="54">
@@ -1355,16 +1355,16 @@
         <v>42522</v>
       </c>
       <c r="B54" t="n">
-        <v>0.8100965821959163</v>
+        <v>0.7291516259314216</v>
       </c>
       <c r="C54" t="n">
-        <v>0.8220806842831399</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D54" t="n">
-        <v>0.5104932049111612</v>
+        <v>0.07851934698335698</v>
       </c>
       <c r="E54" t="n">
-        <v>0.5163659370701217</v>
+        <v>0.2933333333333332</v>
       </c>
     </row>
     <row r="55">
@@ -1372,16 +1372,16 @@
         <v>42552</v>
       </c>
       <c r="B55" t="n">
-        <v>0.8183967831948311</v>
+        <v>0.7135596353022643</v>
       </c>
       <c r="C55" t="n">
-        <v>0.8263757316783266</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D55" t="n">
-        <v>0.3560972505717873</v>
+        <v>0.07622147335176178</v>
       </c>
       <c r="E55" t="n">
-        <v>0.5619120569573679</v>
+        <v>0.2933333333333332</v>
       </c>
     </row>
     <row r="56">
@@ -1389,16 +1389,16 @@
         <v>42583</v>
       </c>
       <c r="B56" t="n">
-        <v>0.8147146482922014</v>
+        <v>0.696689180193885</v>
       </c>
       <c r="C56" t="n">
-        <v>0.818119570113392</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D56" t="n">
-        <v>0.4669182200412889</v>
+        <v>0.1483729308955621</v>
       </c>
       <c r="E56" t="n">
-        <v>0.5786275656828933</v>
+        <v>0.3066666666666666</v>
       </c>
     </row>
     <row r="57">
@@ -1406,16 +1406,16 @@
         <v>42614</v>
       </c>
       <c r="B57" t="n">
-        <v>0.8063220843276583</v>
+        <v>0.6929516378683822</v>
       </c>
       <c r="C57" t="n">
-        <v>0.8237947186483667</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D57" t="n">
-        <v>0.5033182562553414</v>
+        <v>0.1142087580194815</v>
       </c>
       <c r="E57" t="n">
-        <v>0.5104615889743533</v>
+        <v>0.3066666666666666</v>
       </c>
     </row>
     <row r="58">
@@ -1423,16 +1423,16 @@
         <v>42644</v>
       </c>
       <c r="B58" t="n">
-        <v>0.8080478076572463</v>
+        <v>0.7378023525807629</v>
       </c>
       <c r="C58" t="n">
-        <v>0.8165303388546008</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D58" t="n">
-        <v>0.4901319569909405</v>
+        <v>0.2272379146745629</v>
       </c>
       <c r="E58" t="n">
-        <v>0.5415468012974624</v>
+        <v>0.3066666666666666</v>
       </c>
     </row>
     <row r="59">
@@ -1440,16 +1440,16 @@
         <v>42675</v>
       </c>
       <c r="B59" t="n">
-        <v>0.8124965697135286</v>
+        <v>0.7656909454793792</v>
       </c>
       <c r="C59" t="n">
-        <v>0.8169869428260327</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D59" t="n">
-        <v>0.4353786391004341</v>
+        <v>0.2675140607393116</v>
       </c>
       <c r="E59" t="n">
-        <v>0.4469234892367611</v>
+        <v>0.3066666666666666</v>
       </c>
     </row>
     <row r="60">
@@ -1457,16 +1457,16 @@
         <v>42705</v>
       </c>
       <c r="B60" t="n">
-        <v>0.8139368519997429</v>
+        <v>0.7429254332089504</v>
       </c>
       <c r="C60" t="n">
-        <v>0.8207709777432542</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D60" t="n">
-        <v>0.4986856164755484</v>
+        <v>0.177570167950808</v>
       </c>
       <c r="E60" t="n">
-        <v>0.5252535811670093</v>
+        <v>0.3066666666666666</v>
       </c>
     </row>
     <row r="61">
@@ -1474,16 +1474,16 @@
         <v>42736</v>
       </c>
       <c r="B61" t="n">
-        <v>0.8067712217436585</v>
+        <v>0.7323538767891067</v>
       </c>
       <c r="C61" t="n">
-        <v>0.8212166282063189</v>
+        <v>0.7424185238188414</v>
       </c>
       <c r="D61" t="n">
-        <v>0.5700337409100718</v>
+        <v>0.2248148594884905</v>
       </c>
       <c r="E61" t="n">
-        <v>0.6458999251126305</v>
+        <v>0.2933333333333332</v>
       </c>
     </row>
     <row r="62">
@@ -1491,16 +1491,16 @@
         <v>42767</v>
       </c>
       <c r="B62" t="n">
-        <v>0.8182238647215494</v>
+        <v>0.7655461993424407</v>
       </c>
       <c r="C62" t="n">
-        <v>0.8202493854314398</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D62" t="n">
-        <v>0.454856946818932</v>
+        <v>0.1291275243538341</v>
       </c>
       <c r="E62" t="n">
-        <v>0.5859296763199178</v>
+        <v>0.2933333333333332</v>
       </c>
     </row>
     <row r="63">
@@ -1508,16 +1508,16 @@
         <v>42795</v>
       </c>
       <c r="B63" t="n">
-        <v>0.8270024494154147</v>
+        <v>0.7972672935453989</v>
       </c>
       <c r="C63" t="n">
-        <v>0.8173434920035634</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D63" t="n">
-        <v>0.3578150554331625</v>
+        <v>0.09801427958188021</v>
       </c>
       <c r="E63" t="n">
-        <v>0.3562604739452869</v>
+        <v>0.28</v>
       </c>
     </row>
     <row r="64">
@@ -1525,16 +1525,16 @@
         <v>42826</v>
       </c>
       <c r="B64" t="n">
-        <v>0.813441790037817</v>
+        <v>0.6656121123152663</v>
       </c>
       <c r="C64" t="n">
-        <v>0.8198888825138224</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D64" t="n">
-        <v>0.4379823293781138</v>
+        <v>0.08969926805070813</v>
       </c>
       <c r="E64" t="n">
-        <v>0.6272311209685715</v>
+        <v>0.28</v>
       </c>
     </row>
     <row r="65">
@@ -1542,16 +1542,16 @@
         <v>42856</v>
       </c>
       <c r="B65" t="n">
-        <v>0.8005818281819526</v>
+        <v>0.7040975319800307</v>
       </c>
       <c r="C65" t="n">
-        <v>0.8206386649315868</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D65" t="n">
-        <v>0.3433451879440547</v>
+        <v>0.06547998092324661</v>
       </c>
       <c r="E65" t="n">
-        <v>0.4880820644851083</v>
+        <v>0.28</v>
       </c>
     </row>
     <row r="66">
@@ -1559,16 +1559,16 @@
         <v>42887</v>
       </c>
       <c r="B66" t="n">
-        <v>0.8154578610815599</v>
+        <v>0.6848653951925091</v>
       </c>
       <c r="C66" t="n">
-        <v>0.8199435654468733</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D66" t="n">
-        <v>0.410549347079741</v>
+        <v>0.05171211129733437</v>
       </c>
       <c r="E66" t="n">
-        <v>0.5391873865133651</v>
+        <v>0.28</v>
       </c>
     </row>
     <row r="67">
@@ -1576,16 +1576,16 @@
         <v>42917</v>
       </c>
       <c r="B67" t="n">
-        <v>0.8155122669478176</v>
+        <v>0.7631244529995055</v>
       </c>
       <c r="C67" t="n">
-        <v>0.8193649578410942</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D67" t="n">
-        <v>0.3952852113377378</v>
+        <v>0.09963686794957161</v>
       </c>
       <c r="E67" t="n">
-        <v>0.4579019790849181</v>
+        <v>0.28</v>
       </c>
     </row>
     <row r="68">
@@ -1593,16 +1593,16 @@
         <v>42948</v>
       </c>
       <c r="B68" t="n">
-        <v>0.8046915430680994</v>
+        <v>0.7299326898404672</v>
       </c>
       <c r="C68" t="n">
-        <v>0.8175015014051229</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D68" t="n">
-        <v>0.5609150233935125</v>
+        <v>0.1329093331748759</v>
       </c>
       <c r="E68" t="n">
-        <v>0.5177715346724806</v>
+        <v>0.28</v>
       </c>
     </row>
     <row r="69">
@@ -1610,16 +1610,16 @@
         <v>42979</v>
       </c>
       <c r="B69" t="n">
-        <v>0.8335959615893236</v>
+        <v>0.7081952081824725</v>
       </c>
       <c r="C69" t="n">
-        <v>0.8158701824219891</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D69" t="n">
-        <v>0.6199503001817661</v>
+        <v>0.09028407413057055</v>
       </c>
       <c r="E69" t="n">
-        <v>0.5246651788249039</v>
+        <v>0.28</v>
       </c>
     </row>
     <row r="70">
@@ -1627,16 +1627,16 @@
         <v>43009</v>
       </c>
       <c r="B70" t="n">
-        <v>0.7839068529739605</v>
+        <v>0.7249881364338913</v>
       </c>
       <c r="C70" t="n">
-        <v>0.8179849777581502</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D70" t="n">
-        <v>0.4163665091399184</v>
+        <v>0.2330396301547218</v>
       </c>
       <c r="E70" t="n">
-        <v>0.65003305939824</v>
+        <v>0.28</v>
       </c>
     </row>
     <row r="71">
@@ -1644,16 +1644,16 @@
         <v>43040</v>
       </c>
       <c r="B71" t="n">
-        <v>0.8136231473531693</v>
+        <v>0.7218947361669726</v>
       </c>
       <c r="C71" t="n">
-        <v>0.8210746405241639</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D71" t="n">
-        <v>0.5054531287823583</v>
+        <v>0.2859215980242332</v>
       </c>
       <c r="E71" t="n">
-        <v>0.4733556352768684</v>
+        <v>0.28</v>
       </c>
     </row>
     <row r="72">
@@ -1661,16 +1661,16 @@
         <v>43070</v>
       </c>
       <c r="B72" t="n">
-        <v>0.8103141008001655</v>
+        <v>0.7249093672816266</v>
       </c>
       <c r="C72" t="n">
-        <v>0.817819832281291</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D72" t="n">
-        <v>0.4790655403947179</v>
+        <v>0.2095573547602889</v>
       </c>
       <c r="E72" t="n">
-        <v>0.5407224606107112</v>
+        <v>0.2666666666666667</v>
       </c>
     </row>
     <row r="73">
@@ -1678,16 +1678,16 @@
         <v>43101</v>
       </c>
       <c r="B73" t="n">
-        <v>0.8246466423312068</v>
+        <v>0.6609278851124062</v>
       </c>
       <c r="C73" t="n">
-        <v>0.8180028465074485</v>
+        <v>0.2829172649037662</v>
       </c>
       <c r="D73" t="n">
-        <v>0.5579617292651852</v>
+        <v>0.1916099532807182</v>
       </c>
       <c r="E73" t="n">
-        <v>0.6959694050801797</v>
+        <v>0.2533333333333333</v>
       </c>
     </row>
     <row r="74">
@@ -1695,16 +1695,16 @@
         <v>43132</v>
       </c>
       <c r="B74" t="n">
-        <v>0.8330659605477557</v>
+        <v>0.6782284753078431</v>
       </c>
       <c r="C74" t="n">
-        <v>0.8269820793430065</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D74" t="n">
-        <v>0.5115782435314746</v>
+        <v>0.1604063536251415</v>
       </c>
       <c r="E74" t="n">
-        <v>0.6019346898569392</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="75">
@@ -1712,16 +1712,16 @@
         <v>43160</v>
       </c>
       <c r="B75" t="n">
-        <v>0.8075171382937057</v>
+        <v>0.6942504408829298</v>
       </c>
       <c r="C75" t="n">
-        <v>0.8207586939303975</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D75" t="n">
-        <v>0.4066752155894716</v>
+        <v>0.09650908867588781</v>
       </c>
       <c r="E75" t="n">
-        <v>0.6188912423463662</v>
+        <v>0.2266666666666666</v>
       </c>
     </row>
     <row r="76">
@@ -1729,16 +1729,16 @@
         <v>43191</v>
       </c>
       <c r="B76" t="n">
-        <v>0.8102497836714794</v>
+        <v>0.6701090731046015</v>
       </c>
       <c r="C76" t="n">
-        <v>0.8178242058172626</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D76" t="n">
-        <v>0.4864555798421895</v>
+        <v>0.1089714030996026</v>
       </c>
       <c r="E76" t="n">
-        <v>0.5637695601313486</v>
+        <v>0.2133333333333334</v>
       </c>
     </row>
     <row r="77">
@@ -1746,16 +1746,16 @@
         <v>43221</v>
       </c>
       <c r="B77" t="n">
-        <v>0.8183984649936918</v>
+        <v>0.6710208021234072</v>
       </c>
       <c r="C77" t="n">
-        <v>0.824702428264898</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D77" t="n">
-        <v>0.4990037387758953</v>
+        <v>0.02954573504921448</v>
       </c>
       <c r="E77" t="n">
-        <v>0.5790770849706807</v>
+        <v>0.2000000000000001</v>
       </c>
     </row>
     <row r="78">
@@ -1763,16 +1763,16 @@
         <v>43252</v>
       </c>
       <c r="B78" t="n">
-        <v>0.8106440688255686</v>
+        <v>0.6826701985898324</v>
       </c>
       <c r="C78" t="n">
-        <v>0.8202715092558686</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D78" t="n">
-        <v>0.443536424040789</v>
+        <v>0.05045331288529883</v>
       </c>
       <c r="E78" t="n">
-        <v>0.5018084037391228</v>
+        <v>0.2000000000000001</v>
       </c>
     </row>
     <row r="79">
@@ -1780,16 +1780,16 @@
         <v>43282</v>
       </c>
       <c r="B79" t="n">
-        <v>0.8198417357191273</v>
+        <v>0.7197686179088395</v>
       </c>
       <c r="C79" t="n">
-        <v>0.8144787013520314</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D79" t="n">
-        <v>0.4183183667114636</v>
+        <v>0.1246226386877379</v>
       </c>
       <c r="E79" t="n">
-        <v>0.5267517546804865</v>
+        <v>0.2000000000000001</v>
       </c>
     </row>
     <row r="80">
@@ -1797,16 +1797,16 @@
         <v>43313</v>
       </c>
       <c r="B80" t="n">
-        <v>0.7853610245878195</v>
+        <v>0.7217976974583994</v>
       </c>
       <c r="C80" t="n">
-        <v>0.8217106416119848</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D80" t="n">
-        <v>0.4596972479140294</v>
+        <v>0.06500747782321484</v>
       </c>
       <c r="E80" t="n">
-        <v>0.4238883823369072</v>
+        <v>0.1866666666666666</v>
       </c>
     </row>
     <row r="81">
@@ -1814,16 +1814,16 @@
         <v>43344</v>
       </c>
       <c r="B81" t="n">
-        <v>0.824129043682934</v>
+        <v>0.7001108841853869</v>
       </c>
       <c r="C81" t="n">
-        <v>0.8157033295949545</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D81" t="n">
-        <v>0.4715287686595205</v>
+        <v>0.1149935143650011</v>
       </c>
       <c r="E81" t="n">
-        <v>0.5989646552265293</v>
+        <v>0.1866666666666666</v>
       </c>
     </row>
     <row r="82">
@@ -1831,16 +1831,16 @@
         <v>43374</v>
       </c>
       <c r="B82" t="n">
-        <v>0.819552886792289</v>
+        <v>0.6507496823181886</v>
       </c>
       <c r="C82" t="n">
-        <v>0.818528860816482</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D82" t="n">
-        <v>0.4961603152117828</v>
+        <v>0.1838403990939367</v>
       </c>
       <c r="E82" t="n">
-        <v>0.529738074941725</v>
+        <v>0.2000000000000001</v>
       </c>
     </row>
     <row r="83">
@@ -1848,16 +1848,16 @@
         <v>43405</v>
       </c>
       <c r="B83" t="n">
-        <v>0.8179852778074733</v>
+        <v>0.6708553423466506</v>
       </c>
       <c r="C83" t="n">
-        <v>0.8159579012005663</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D83" t="n">
-        <v>0.3415997683456339</v>
+        <v>0.3205300384075511</v>
       </c>
       <c r="E83" t="n">
-        <v>0.5768185843840613</v>
+        <v>0.2000000000000001</v>
       </c>
     </row>
     <row r="84">
@@ -1865,16 +1865,16 @@
         <v>43435</v>
       </c>
       <c r="B84" t="n">
-        <v>0.8101511910185669</v>
+        <v>0.6741237090032509</v>
       </c>
       <c r="C84" t="n">
-        <v>0.8191864508538729</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D84" t="n">
-        <v>0.3600564217250121</v>
+        <v>0.2166467015686408</v>
       </c>
       <c r="E84" t="n">
-        <v>0.5533437486194742</v>
+        <v>0.2000000000000001</v>
       </c>
     </row>
     <row r="85">
@@ -1882,16 +1882,16 @@
         <v>43466</v>
       </c>
       <c r="B85" t="n">
-        <v>0.7973139801202804</v>
+        <v>0.6257482852633167</v>
       </c>
       <c r="C85" t="n">
-        <v>0.8238482704331076</v>
+        <v>0.4480363918298151</v>
       </c>
       <c r="D85" t="n">
-        <v>0.3647174717258458</v>
+        <v>0.21112718323324</v>
       </c>
       <c r="E85" t="n">
-        <v>0.5077104628409661</v>
+        <v>0.1866666666666666</v>
       </c>
     </row>
     <row r="86">
@@ -1899,16 +1899,16 @@
         <v>43497</v>
       </c>
       <c r="B86" t="n">
-        <v>0.8196116871088801</v>
+        <v>0.5994275175881978</v>
       </c>
       <c r="C86" t="n">
-        <v>0.8115732332084368</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D86" t="n">
-        <v>0.5038792710841919</v>
+        <v>0.1460497254908808</v>
       </c>
       <c r="E86" t="n">
-        <v>0.463085594596551</v>
+        <v>0.1733333333333333</v>
       </c>
     </row>
     <row r="87">
@@ -1916,16 +1916,16 @@
         <v>43525</v>
       </c>
       <c r="B87" t="n">
-        <v>0.8018329244093183</v>
+        <v>0.581022867246383</v>
       </c>
       <c r="C87" t="n">
-        <v>0.820830340412487</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D87" t="n">
-        <v>0.5913563343395413</v>
+        <v>0.1070097978083133</v>
       </c>
       <c r="E87" t="n">
-        <v>0.5229124522593995</v>
+        <v>0.1599999999999999</v>
       </c>
     </row>
     <row r="88">
@@ -1933,16 +1933,16 @@
         <v>43556</v>
       </c>
       <c r="B88" t="n">
-        <v>0.8045367245601444</v>
+        <v>0.6316208854271055</v>
       </c>
       <c r="C88" t="n">
-        <v>0.8213716492306352</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D88" t="n">
-        <v>0.5446092017417534</v>
+        <v>0.05311231739864392</v>
       </c>
       <c r="E88" t="n">
-        <v>0.6567251848649527</v>
+        <v>0.1466666666666666</v>
       </c>
     </row>
     <row r="89">
@@ -1950,16 +1950,16 @@
         <v>43586</v>
       </c>
       <c r="B89" t="n">
-        <v>0.8113212842232385</v>
+        <v>0.6685910221009247</v>
       </c>
       <c r="C89" t="n">
-        <v>0.8148626901969781</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D89" t="n">
-        <v>0.4097728513891348</v>
+        <v>0.01913603512735493</v>
       </c>
       <c r="E89" t="n">
-        <v>0.5053976234202497</v>
+        <v>0.1466666666666666</v>
       </c>
     </row>
     <row r="90">
@@ -1967,16 +1967,16 @@
         <v>43617</v>
       </c>
       <c r="B90" t="n">
-        <v>0.8186221843914154</v>
+        <v>0.6681686659419835</v>
       </c>
       <c r="C90" t="n">
-        <v>0.8185509208111434</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D90" t="n">
-        <v>0.38649153885636</v>
+        <v>0.1362984965529224</v>
       </c>
       <c r="E90" t="n">
-        <v>0.5937308945445607</v>
+        <v>0.1466666666666666</v>
       </c>
     </row>
     <row r="91">
@@ -1984,16 +1984,16 @@
         <v>43647</v>
       </c>
       <c r="B91" t="n">
-        <v>0.8189620174086807</v>
+        <v>0.7282777117401232</v>
       </c>
       <c r="C91" t="n">
-        <v>0.8154117944889092</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D91" t="n">
-        <v>0.4792752537025191</v>
+        <v>0.08302764632481906</v>
       </c>
       <c r="E91" t="n">
-        <v>0.5339395888648751</v>
+        <v>0.1466666666666666</v>
       </c>
     </row>
     <row r="92">
@@ -2001,16 +2001,16 @@
         <v>43678</v>
       </c>
       <c r="B92" t="n">
-        <v>0.8154828077055877</v>
+        <v>0.7451096573892022</v>
       </c>
       <c r="C92" t="n">
-        <v>0.8209335594642065</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D92" t="n">
-        <v>0.4312301472581591</v>
+        <v>0.1233335959615849</v>
       </c>
       <c r="E92" t="n">
-        <v>0.4964481869322119</v>
+        <v>0.1466666666666666</v>
       </c>
     </row>
     <row r="93">
@@ -2018,16 +2018,16 @@
         <v>43709</v>
       </c>
       <c r="B93" t="n">
-        <v>0.8241791552854203</v>
+        <v>0.7396588655575723</v>
       </c>
       <c r="C93" t="n">
-        <v>0.8200016738212278</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D93" t="n">
-        <v>0.4565441355295847</v>
+        <v>0.1225453046803383</v>
       </c>
       <c r="E93" t="n">
-        <v>0.4590688056041738</v>
+        <v>0.1333333333333334</v>
       </c>
     </row>
     <row r="94">
@@ -2035,16 +2035,16 @@
         <v>43739</v>
       </c>
       <c r="B94" t="n">
-        <v>0.8126319742663987</v>
+        <v>0.6526932992257946</v>
       </c>
       <c r="C94" t="n">
-        <v>0.8171276262622229</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D94" t="n">
-        <v>0.5099701165816628</v>
+        <v>0.2005696490265312</v>
       </c>
       <c r="E94" t="n">
-        <v>0.5335409584901164</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="95">
@@ -2052,16 +2052,16 @@
         <v>43770</v>
       </c>
       <c r="B95" t="n">
-        <v>0.8124937237162303</v>
+        <v>0.676616113422199</v>
       </c>
       <c r="C95" t="n">
-        <v>0.8202781681486746</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D95" t="n">
-        <v>0.4682875810744797</v>
+        <v>0.3435755222492816</v>
       </c>
       <c r="E95" t="n">
-        <v>0.4242667995674879</v>
+        <v>0.1066666666666667</v>
       </c>
     </row>
     <row r="96">
@@ -2069,16 +2069,16 @@
         <v>43800</v>
       </c>
       <c r="B96" t="n">
-        <v>0.8132794396938479</v>
+        <v>0.6456108962880549</v>
       </c>
       <c r="C96" t="n">
-        <v>0.8161275251408611</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D96" t="n">
-        <v>0.4666626050633214</v>
+        <v>0.2087906175649007</v>
       </c>
       <c r="E96" t="n">
-        <v>0.610186243029978</v>
+        <v>0.1066666666666667</v>
       </c>
     </row>
     <row r="97">
@@ -2086,16 +2086,16 @@
         <v>43831</v>
       </c>
       <c r="B97" t="n">
-        <v>0.7973372499006984</v>
+        <v>0.5518712805846355</v>
       </c>
       <c r="C97" t="n">
-        <v>0.8246147103723622</v>
+        <v>1</v>
       </c>
       <c r="D97" t="n">
-        <v>0.4562957516250217</v>
+        <v>0.1689552854503726</v>
       </c>
       <c r="E97" t="n">
-        <v>0.5996197569036025</v>
+        <v>0.1066666666666667</v>
       </c>
     </row>
     <row r="98">
@@ -2103,16 +2103,16 @@
         <v>43862</v>
       </c>
       <c r="B98" t="n">
-        <v>0.8137453876417202</v>
+        <v>0.5626205813947409</v>
       </c>
       <c r="C98" t="n">
-        <v>0.8223618312985181</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D98" t="n">
-        <v>0.439059555797408</v>
+        <v>0.1138347626910712</v>
       </c>
       <c r="E98" t="n">
-        <v>0.5672520769960205</v>
+        <v>0.1066666666666667</v>
       </c>
     </row>
     <row r="99">
@@ -2120,16 +2120,16 @@
         <v>43891</v>
       </c>
       <c r="B99" t="n">
-        <v>0.6969692592429803</v>
+        <v>0.6138800449416087</v>
       </c>
       <c r="C99" t="n">
-        <v>0.7600573027159682</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D99" t="n">
-        <v>0.2262743642876197</v>
+        <v>0.1588027269158376</v>
       </c>
       <c r="E99" t="n">
-        <v>0.3475686660349202</v>
+        <v>0.1066666666666667</v>
       </c>
     </row>
     <row r="100">
@@ -2137,16 +2137,16 @@
         <v>43922</v>
       </c>
       <c r="B100" t="n">
-        <v>0</v>
+        <v>0.1854891697657058</v>
       </c>
       <c r="C100" t="n">
-        <v>0</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D100" t="n">
-        <v>0</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="E100" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="101">
@@ -2154,16 +2154,16 @@
         <v>43952</v>
       </c>
       <c r="B101" t="n">
-        <v>0.9569070071883189</v>
+        <v>0.06373611065004237</v>
       </c>
       <c r="C101" t="n">
-        <v>0.9232072175524301</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D101" t="n">
-        <v>0.3522132825430839</v>
+        <v>0.1308972280643041</v>
       </c>
       <c r="E101" t="n">
-        <v>0.5280927989299551</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102">
@@ -2171,16 +2171,16 @@
         <v>43983</v>
       </c>
       <c r="B102" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C102" t="n">
-        <v>1</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D102" t="n">
-        <v>0.6138188260274466</v>
+        <v>0.1087147453695275</v>
       </c>
       <c r="E102" t="n">
-        <v>0.5961687781641267</v>
+        <v>0.9200000000000002</v>
       </c>
     </row>
     <row r="103">
@@ -2188,16 +2188,16 @@
         <v>44013</v>
       </c>
       <c r="B103" t="n">
-        <v>0.8619915693855537</v>
+        <v>0.9957808963720891</v>
       </c>
       <c r="C103" t="n">
-        <v>0.8704398225170659</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D103" t="n">
-        <v>0.6223428498919439</v>
+        <v>0.09586263734510431</v>
       </c>
       <c r="E103" t="n">
-        <v>0.7150513986441051</v>
+        <v>0.9066666666666665</v>
       </c>
     </row>
     <row r="104">
@@ -2205,16 +2205,16 @@
         <v>44044</v>
       </c>
       <c r="B104" t="n">
-        <v>0.9301592416903756</v>
+        <v>0.986287117004685</v>
       </c>
       <c r="C104" t="n">
-        <v>0.8813465190089401</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D104" t="n">
-        <v>0.568632768710604</v>
+        <v>0.0358803669984015</v>
       </c>
       <c r="E104" t="n">
-        <v>0.6997994837507728</v>
+        <v>0.4533333333333334</v>
       </c>
     </row>
     <row r="105">
@@ -2222,16 +2222,16 @@
         <v>44075</v>
       </c>
       <c r="B105" t="n">
-        <v>0.8220104815944788</v>
+        <v>0.997992660056092</v>
       </c>
       <c r="C105" t="n">
-        <v>0.8502188608049476</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D105" t="n">
-        <v>0.4905468607131919</v>
+        <v>0.01094657111090652</v>
       </c>
       <c r="E105" t="n">
-        <v>0.5652936534579119</v>
+        <v>0.4399999999999999</v>
       </c>
     </row>
     <row r="106">
@@ -2239,16 +2239,16 @@
         <v>44105</v>
       </c>
       <c r="B106" t="n">
-        <v>0.8854473545587337</v>
+        <v>0.8907890136135153</v>
       </c>
       <c r="C106" t="n">
-        <v>0.8405250090915963</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D106" t="n">
-        <v>0.4091997879257664</v>
+        <v>0.02270134778887667</v>
       </c>
       <c r="E106" t="n">
-        <v>0.4323131678084687</v>
+        <v>0.3866666666666666</v>
       </c>
     </row>
     <row r="107">
@@ -2256,16 +2256,16 @@
         <v>44136</v>
       </c>
       <c r="B107" t="n">
-        <v>0.809529527014256</v>
+        <v>0.8904422706182485</v>
       </c>
       <c r="C107" t="n">
-        <v>0.8226838610176903</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D107" t="n">
-        <v>0.4466437111373774</v>
+        <v>0.1670730428916797</v>
       </c>
       <c r="E107" t="n">
-        <v>0.4264583262667098</v>
+        <v>0.3733333333333333</v>
       </c>
     </row>
     <row r="108">
@@ -2273,16 +2273,16 @@
         <v>44166</v>
       </c>
       <c r="B108" t="n">
-        <v>0.8080962408847309</v>
+        <v>0.8231783316580503</v>
       </c>
       <c r="C108" t="n">
-        <v>0.801936736537891</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D108" t="n">
-        <v>0.5321018246348093</v>
+        <v>0.164798398250988</v>
       </c>
       <c r="E108" t="n">
-        <v>0.7123305533138278</v>
+        <v>0.3866666666666666</v>
       </c>
     </row>
     <row r="109">
@@ -2290,16 +2290,16 @@
         <v>44197</v>
       </c>
       <c r="B109" t="n">
-        <v>0.8037985530107958</v>
+        <v>0.8532357987090885</v>
       </c>
       <c r="C109" t="n">
-        <v>0.8316384498028809</v>
+        <v>0.3638093175350565</v>
       </c>
       <c r="D109" t="n">
-        <v>0.4943928131909315</v>
+        <v>0.1437737888704036</v>
       </c>
       <c r="E109" t="n">
-        <v>0.6997077357536218</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="110">
@@ -2307,16 +2307,16 @@
         <v>44228</v>
       </c>
       <c r="B110" t="n">
-        <v>0.8186046173234472</v>
+        <v>0.8578370890224951</v>
       </c>
       <c r="C110" t="n">
-        <v>0.8347112478477754</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D110" t="n">
-        <v>0.5855552089591999</v>
+        <v>0.06560191823470822</v>
       </c>
       <c r="E110" t="n">
-        <v>0.5605591914330481</v>
+        <v>0.3466666666666667</v>
       </c>
     </row>
     <row r="111">
@@ -2324,16 +2324,16 @@
         <v>44256</v>
       </c>
       <c r="B111" t="n">
-        <v>0.8259506443671929</v>
+        <v>0.8148460278859364</v>
       </c>
       <c r="C111" t="n">
-        <v>0.8426814771918714</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D111" t="n">
-        <v>0.6801679785195373</v>
+        <v>0.08684425968862515</v>
       </c>
       <c r="E111" t="n">
-        <v>0.7989657965682966</v>
+        <v>0.3466666666666667</v>
       </c>
     </row>
     <row r="112">
@@ -2341,16 +2341,16 @@
         <v>44287</v>
       </c>
       <c r="B112" t="n">
-        <v>0.8215175625321907</v>
+        <v>0.7908049676540101</v>
       </c>
       <c r="C112" t="n">
-        <v>0.8233982244678987</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D112" t="n">
-        <v>0.681290936005489</v>
+        <v>0.08858162541534628</v>
       </c>
       <c r="E112" t="n">
-        <v>0.9999999999999999</v>
+        <v>0.3466666666666667</v>
       </c>
     </row>
     <row r="113">
@@ -2358,16 +2358,16 @@
         <v>44317</v>
       </c>
       <c r="B113" t="n">
-        <v>0.8177091421539534</v>
+        <v>0.7924606105483781</v>
       </c>
       <c r="C113" t="n">
-        <v>0.8308942638373007</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D113" t="n">
-        <v>0.7097890436050871</v>
+        <v>0.06723860588676225</v>
       </c>
       <c r="E113" t="n">
-        <v>0.89195293622401</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="114">
@@ -2375,16 +2375,16 @@
         <v>44348</v>
       </c>
       <c r="B114" t="n">
-        <v>0.8139240932155383</v>
+        <v>0.7829494782701982</v>
       </c>
       <c r="C114" t="n">
-        <v>0.8388879424853678</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D114" t="n">
-        <v>0.7918698206865462</v>
+        <v>0.05680511272516202</v>
       </c>
       <c r="E114" t="n">
-        <v>0.8578031108107756</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="115">
@@ -2392,16 +2392,16 @@
         <v>44378</v>
       </c>
       <c r="B115" t="n">
-        <v>0.8447262678280361</v>
+        <v>0.8191143053132359</v>
       </c>
       <c r="C115" t="n">
-        <v>0.8416470585126722</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D115" t="n">
-        <v>0.5933676549433829</v>
+        <v>0</v>
       </c>
       <c r="E115" t="n">
-        <v>0.7748220802009727</v>
+        <v>0.28</v>
       </c>
     </row>
     <row r="116">
@@ -2409,16 +2409,16 @@
         <v>44409</v>
       </c>
       <c r="B116" t="n">
-        <v>0.8216318148412766</v>
+        <v>0.8261995895600249</v>
       </c>
       <c r="C116" t="n">
-        <v>0.8374910264999796</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D116" t="n">
-        <v>0.5369842896455852</v>
+        <v>0.04715612640420984</v>
       </c>
       <c r="E116" t="n">
-        <v>0.7137546556932208</v>
+        <v>0.2533333333333333</v>
       </c>
     </row>
     <row r="117">
@@ -2426,16 +2426,16 @@
         <v>44440</v>
       </c>
       <c r="B117" t="n">
-        <v>0.829324685465715</v>
+        <v>0.8364256009224009</v>
       </c>
       <c r="C117" t="n">
-        <v>0.8333904031509844</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D117" t="n">
-        <v>0.5733056891296506</v>
+        <v>0.3121435017940396</v>
       </c>
       <c r="E117" t="n">
-        <v>0.5994127930325178</v>
+        <v>0.2000000000000001</v>
       </c>
     </row>
     <row r="118">
@@ -2443,16 +2443,16 @@
         <v>44470</v>
       </c>
       <c r="B118" t="n">
-        <v>0.8248883981973458</v>
+        <v>0.8730233769786331</v>
       </c>
       <c r="C118" t="n">
-        <v>0.8417035358198151</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D118" t="n">
-        <v>0.7869501147721993</v>
+        <v>0.04351923620271793</v>
       </c>
       <c r="E118" t="n">
-        <v>0.7882130413787518</v>
+        <v>0.1733333333333333</v>
       </c>
     </row>
     <row r="119">
@@ -2460,16 +2460,16 @@
         <v>44501</v>
       </c>
       <c r="B119" t="n">
-        <v>0.8454799427581161</v>
+        <v>0.8622525100974402</v>
       </c>
       <c r="C119" t="n">
-        <v>0.8353271160933808</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D119" t="n">
-        <v>0.7086646182002438</v>
+        <v>0.1678222464745851</v>
       </c>
       <c r="E119" t="n">
-        <v>0.8911020815703479</v>
+        <v>0.1466666666666666</v>
       </c>
     </row>
     <row r="120">
@@ -2477,16 +2477,16 @@
         <v>44531</v>
       </c>
       <c r="B120" t="n">
-        <v>0.8253004314759759</v>
+        <v>0.8687237521401663</v>
       </c>
       <c r="C120" t="n">
-        <v>0.833561803676217</v>
+        <v>0.6709307585010981</v>
       </c>
       <c r="D120" t="n">
-        <v>0.6505070675988471</v>
+        <v>0.2223187555156418</v>
       </c>
       <c r="E120" t="n">
-        <v>0.9171476396221474</v>
+        <v>0.1466666666666666</v>
       </c>
     </row>
     <row r="121">
@@ -2494,16 +2494,16 @@
         <v>44562</v>
       </c>
       <c r="B121" t="n">
-        <v>0.8417655800512969</v>
+        <v>0.6200002576047271</v>
       </c>
       <c r="C121" t="n">
-        <v>0.8258912572247243</v>
+        <v>0</v>
       </c>
       <c r="D121" t="n">
-        <v>0.6833060359507753</v>
+        <v>0.1447208415238817</v>
       </c>
       <c r="E121" t="n">
-        <v>0.849716319317243</v>
+        <v>0.1599999999999999</v>
       </c>
     </row>
     <row r="122">
@@ -2511,16 +2511,16 @@
         <v>44593</v>
       </c>
       <c r="B122" t="n">
-        <v>0.8225231991975527</v>
+        <v>0.609954600126257</v>
       </c>
       <c r="C122" t="n">
-        <v>0.8457818859679205</v>
+        <v>0</v>
       </c>
       <c r="D122" t="n">
-        <v>0.7548506731960245</v>
+        <v>0.09447220795576386</v>
       </c>
       <c r="E122" t="n">
-        <v>0.7502070432831904</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="123">
@@ -2528,16 +2528,16 @@
         <v>44621</v>
       </c>
       <c r="B123" t="n">
-        <v>0.8314178054745589</v>
+        <v>0.5548641901343707</v>
       </c>
       <c r="C123" t="n">
-        <v>0.8276147347747844</v>
+        <v>0</v>
       </c>
       <c r="D123" t="n">
-        <v>0.9618970566512602</v>
+        <v>0.08647078820209839</v>
       </c>
       <c r="E123" t="n">
-        <v>0.7505054023472113</v>
+        <v>0.06666666666666665</v>
       </c>
     </row>
     <row r="124">
@@ -2545,16 +2545,16 @@
         <v>44652</v>
       </c>
       <c r="B124" t="n">
-        <v>0.7954831318683658</v>
+        <v>1</v>
       </c>
       <c r="C124" t="n">
-        <v>0.8217095570311057</v>
+        <v>0</v>
       </c>
       <c r="D124" t="n">
-        <v>0.5362716851339961</v>
+        <v>0.04582352119832925</v>
       </c>
       <c r="E124" t="n">
-        <v>0.6969382685085479</v>
+        <v>0.05333333333333334</v>
       </c>
     </row>
     <row r="125">
@@ -2562,16 +2562,16 @@
         <v>44682</v>
       </c>
       <c r="B125" t="n">
-        <v>0.8174440166948352</v>
+        <v>0.9297531507320034</v>
       </c>
       <c r="C125" t="n">
-        <v>0.8257191154752621</v>
+        <v>0</v>
       </c>
       <c r="D125" t="n">
-        <v>0.8373213481418396</v>
+        <v>0.05608747404409839</v>
       </c>
       <c r="E125" t="n">
-        <v>0.7574979756451474</v>
+        <v>0.02666666666666662</v>
       </c>
     </row>
     <row r="126">
@@ -2579,16 +2579,16 @@
         <v>44713</v>
       </c>
       <c r="B126" t="n">
-        <v>0.7989289927695611</v>
+        <v>0.8634609793751494</v>
       </c>
       <c r="C126" t="n">
-        <v>0.8259061849629872</v>
+        <v>0</v>
       </c>
       <c r="D126" t="n">
-        <v>1</v>
+        <v>0.08795774559793565</v>
       </c>
       <c r="E126" t="n">
-        <v>0.9976709862639096</v>
+        <v>0.02666666666666662</v>
       </c>
     </row>
     <row r="127">
@@ -2596,16 +2596,16 @@
         <v>44743</v>
       </c>
       <c r="B127" t="n">
-        <v>0.8140641755195509</v>
+        <v>0.7021570233960444</v>
       </c>
       <c r="C127" t="n">
-        <v>0.8330763197266476</v>
+        <v>0</v>
       </c>
       <c r="D127" t="n">
-        <v>0.3707296219929684</v>
+        <v>0.1160682841149195</v>
       </c>
       <c r="E127" t="n">
-        <v>0.4732109611094415</v>
+        <v>0.01333333333333331</v>
       </c>
     </row>
     <row r="128">
@@ -2613,16 +2613,16 @@
         <v>44774</v>
       </c>
       <c r="B128" t="n">
-        <v>0.8208919451701608</v>
+        <v>0.6461232398439661</v>
       </c>
       <c r="C128" t="n">
-        <v>0.8251705550787586</v>
+        <v>0</v>
       </c>
       <c r="D128" t="n">
-        <v>0.4356150255383813</v>
+        <v>0.1099469675794406</v>
       </c>
       <c r="E128" t="n">
-        <v>0.9236480720229472</v>
+        <v>0.02666666666666662</v>
       </c>
     </row>
     <row r="129">
@@ -2630,16 +2630,16 @@
         <v>44805</v>
       </c>
       <c r="B129" t="n">
-        <v>0.8120903226948355</v>
+        <v>0.6343537641550312</v>
       </c>
       <c r="C129" t="n">
-        <v>0.8250688681905269</v>
+        <v>0</v>
       </c>
       <c r="D129" t="n">
-        <v>0.5617259035703712</v>
+        <v>0.08860265721166044</v>
       </c>
       <c r="E129" t="n">
-        <v>0.8420785671979352</v>
+        <v>0</v>
       </c>
     </row>
     <row r="130">
@@ -2647,16 +2647,16 @@
         <v>44835</v>
       </c>
       <c r="B130" t="n">
-        <v>0.7984613780182788</v>
+        <v>0.5624905753281257</v>
       </c>
       <c r="C130" t="n">
-        <v>0.8241011740306265</v>
+        <v>0</v>
       </c>
       <c r="D130" t="n">
-        <v>0.5863861258720136</v>
+        <v>0.2383948984827638</v>
       </c>
       <c r="E130" t="n">
-        <v>0.6907366034206341</v>
+        <v>0</v>
       </c>
     </row>
     <row r="131">
@@ -2664,16 +2664,16 @@
         <v>44866</v>
       </c>
       <c r="B131" t="n">
-        <v>0.8047628919116875</v>
+        <v>0.6056468360159089</v>
       </c>
       <c r="C131" t="n">
-        <v>0.8228511729719241</v>
+        <v>0</v>
       </c>
       <c r="D131" t="n">
-        <v>0.4252858022654106</v>
+        <v>0.3146825776440439</v>
       </c>
       <c r="E131" t="n">
-        <v>0.6069710135351849</v>
+        <v>0</v>
       </c>
     </row>
     <row r="132">
@@ -2681,16 +2681,16 @@
         <v>44896</v>
       </c>
       <c r="B132" t="n">
-        <v>0.8305827208491328</v>
+        <v>0.6123202873230487</v>
       </c>
       <c r="C132" t="n">
-        <v>0.8209963916862013</v>
+        <v>0</v>
       </c>
       <c r="D132" t="n">
         <v>0</v>
       </c>
       <c r="E132" t="n">
-        <v>0.7567272753999312</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>